<commit_message>
resultados en carpetas segun leadtime
</commit_message>
<xml_diff>
--- a/pronostico_demanda/excel_branches/branch0(2).xlsx
+++ b/pronostico_demanda/excel_branches/branch0(2).xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6564"/>
+  <dimension ref="A1:E6596"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -111688,7 +111688,7 @@
         <v>121</v>
       </c>
       <c r="E6547">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6548" spans="1:5">
@@ -111722,7 +111722,7 @@
         <v>121</v>
       </c>
       <c r="E6549">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6550" spans="1:5">
@@ -111739,7 +111739,7 @@
         <v>121</v>
       </c>
       <c r="E6550">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6551" spans="1:5">
@@ -111756,7 +111756,7 @@
         <v>121</v>
       </c>
       <c r="E6551">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6552" spans="1:5">
@@ -111773,7 +111773,7 @@
         <v>121</v>
       </c>
       <c r="E6552">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6553" spans="1:5">
@@ -111807,7 +111807,7 @@
         <v>121</v>
       </c>
       <c r="E6554">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6555" spans="1:5">
@@ -111824,7 +111824,7 @@
         <v>121</v>
       </c>
       <c r="E6555">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6556" spans="1:5">
@@ -111841,7 +111841,7 @@
         <v>121</v>
       </c>
       <c r="E6556">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6557" spans="1:5">
@@ -111858,7 +111858,7 @@
         <v>121</v>
       </c>
       <c r="E6557">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6558" spans="1:5">
@@ -111977,6 +111977,550 @@
         <v>121</v>
       </c>
       <c r="E6564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6565" spans="1:5">
+      <c r="A6565">
+        <v>6563</v>
+      </c>
+      <c r="B6565">
+        <v>0</v>
+      </c>
+      <c r="C6565">
+        <v>236</v>
+      </c>
+      <c r="D6565">
+        <v>121</v>
+      </c>
+      <c r="E6565">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6566" spans="1:5">
+      <c r="A6566">
+        <v>6564</v>
+      </c>
+      <c r="B6566">
+        <v>0</v>
+      </c>
+      <c r="C6566">
+        <v>237</v>
+      </c>
+      <c r="D6566">
+        <v>121</v>
+      </c>
+      <c r="E6566">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6567" spans="1:5">
+      <c r="A6567">
+        <v>6565</v>
+      </c>
+      <c r="B6567">
+        <v>0</v>
+      </c>
+      <c r="C6567">
+        <v>238</v>
+      </c>
+      <c r="D6567">
+        <v>121</v>
+      </c>
+      <c r="E6567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6568" spans="1:5">
+      <c r="A6568">
+        <v>6566</v>
+      </c>
+      <c r="B6568">
+        <v>0</v>
+      </c>
+      <c r="C6568">
+        <v>239</v>
+      </c>
+      <c r="D6568">
+        <v>121</v>
+      </c>
+      <c r="E6568">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6569" spans="1:5">
+      <c r="A6569">
+        <v>6567</v>
+      </c>
+      <c r="B6569">
+        <v>0</v>
+      </c>
+      <c r="C6569">
+        <v>240</v>
+      </c>
+      <c r="D6569">
+        <v>121</v>
+      </c>
+      <c r="E6569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6570" spans="1:5">
+      <c r="A6570">
+        <v>6568</v>
+      </c>
+      <c r="B6570">
+        <v>0</v>
+      </c>
+      <c r="C6570">
+        <v>241</v>
+      </c>
+      <c r="D6570">
+        <v>121</v>
+      </c>
+      <c r="E6570">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6571" spans="1:5">
+      <c r="A6571">
+        <v>6569</v>
+      </c>
+      <c r="B6571">
+        <v>0</v>
+      </c>
+      <c r="C6571">
+        <v>242</v>
+      </c>
+      <c r="D6571">
+        <v>121</v>
+      </c>
+      <c r="E6571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6572" spans="1:5">
+      <c r="A6572">
+        <v>6570</v>
+      </c>
+      <c r="B6572">
+        <v>0</v>
+      </c>
+      <c r="C6572">
+        <v>243</v>
+      </c>
+      <c r="D6572">
+        <v>121</v>
+      </c>
+      <c r="E6572">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6573" spans="1:5">
+      <c r="A6573">
+        <v>6571</v>
+      </c>
+      <c r="B6573">
+        <v>0</v>
+      </c>
+      <c r="C6573">
+        <v>244</v>
+      </c>
+      <c r="D6573">
+        <v>121</v>
+      </c>
+      <c r="E6573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6574" spans="1:5">
+      <c r="A6574">
+        <v>6572</v>
+      </c>
+      <c r="B6574">
+        <v>0</v>
+      </c>
+      <c r="C6574">
+        <v>245</v>
+      </c>
+      <c r="D6574">
+        <v>121</v>
+      </c>
+      <c r="E6574">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6575" spans="1:5">
+      <c r="A6575">
+        <v>6573</v>
+      </c>
+      <c r="B6575">
+        <v>0</v>
+      </c>
+      <c r="C6575">
+        <v>246</v>
+      </c>
+      <c r="D6575">
+        <v>121</v>
+      </c>
+      <c r="E6575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6576" spans="1:5">
+      <c r="A6576">
+        <v>6574</v>
+      </c>
+      <c r="B6576">
+        <v>0</v>
+      </c>
+      <c r="C6576">
+        <v>247</v>
+      </c>
+      <c r="D6576">
+        <v>121</v>
+      </c>
+      <c r="E6576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6577" spans="1:5">
+      <c r="A6577">
+        <v>6575</v>
+      </c>
+      <c r="B6577">
+        <v>0</v>
+      </c>
+      <c r="C6577">
+        <v>248</v>
+      </c>
+      <c r="D6577">
+        <v>121</v>
+      </c>
+      <c r="E6577">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6578" spans="1:5">
+      <c r="A6578">
+        <v>6576</v>
+      </c>
+      <c r="B6578">
+        <v>0</v>
+      </c>
+      <c r="C6578">
+        <v>249</v>
+      </c>
+      <c r="D6578">
+        <v>121</v>
+      </c>
+      <c r="E6578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6579" spans="1:5">
+      <c r="A6579">
+        <v>6577</v>
+      </c>
+      <c r="B6579">
+        <v>0</v>
+      </c>
+      <c r="C6579">
+        <v>250</v>
+      </c>
+      <c r="D6579">
+        <v>121</v>
+      </c>
+      <c r="E6579">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6580" spans="1:5">
+      <c r="A6580">
+        <v>6578</v>
+      </c>
+      <c r="B6580">
+        <v>0</v>
+      </c>
+      <c r="C6580">
+        <v>251</v>
+      </c>
+      <c r="D6580">
+        <v>121</v>
+      </c>
+      <c r="E6580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6581" spans="1:5">
+      <c r="A6581">
+        <v>6579</v>
+      </c>
+      <c r="B6581">
+        <v>0</v>
+      </c>
+      <c r="C6581">
+        <v>252</v>
+      </c>
+      <c r="D6581">
+        <v>121</v>
+      </c>
+      <c r="E6581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6582" spans="1:5">
+      <c r="A6582">
+        <v>6580</v>
+      </c>
+      <c r="B6582">
+        <v>0</v>
+      </c>
+      <c r="C6582">
+        <v>253</v>
+      </c>
+      <c r="D6582">
+        <v>121</v>
+      </c>
+      <c r="E6582">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6583" spans="1:5">
+      <c r="A6583">
+        <v>6581</v>
+      </c>
+      <c r="B6583">
+        <v>0</v>
+      </c>
+      <c r="C6583">
+        <v>254</v>
+      </c>
+      <c r="D6583">
+        <v>121</v>
+      </c>
+      <c r="E6583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6584" spans="1:5">
+      <c r="A6584">
+        <v>6582</v>
+      </c>
+      <c r="B6584">
+        <v>0</v>
+      </c>
+      <c r="C6584">
+        <v>255</v>
+      </c>
+      <c r="D6584">
+        <v>121</v>
+      </c>
+      <c r="E6584">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6585" spans="1:5">
+      <c r="A6585">
+        <v>6583</v>
+      </c>
+      <c r="B6585">
+        <v>0</v>
+      </c>
+      <c r="C6585">
+        <v>256</v>
+      </c>
+      <c r="D6585">
+        <v>121</v>
+      </c>
+      <c r="E6585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6586" spans="1:5">
+      <c r="A6586">
+        <v>6584</v>
+      </c>
+      <c r="B6586">
+        <v>0</v>
+      </c>
+      <c r="C6586">
+        <v>257</v>
+      </c>
+      <c r="D6586">
+        <v>121</v>
+      </c>
+      <c r="E6586">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6587" spans="1:5">
+      <c r="A6587">
+        <v>6585</v>
+      </c>
+      <c r="B6587">
+        <v>0</v>
+      </c>
+      <c r="C6587">
+        <v>258</v>
+      </c>
+      <c r="D6587">
+        <v>121</v>
+      </c>
+      <c r="E6587">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6588" spans="1:5">
+      <c r="A6588">
+        <v>6586</v>
+      </c>
+      <c r="B6588">
+        <v>0</v>
+      </c>
+      <c r="C6588">
+        <v>259</v>
+      </c>
+      <c r="D6588">
+        <v>121</v>
+      </c>
+      <c r="E6588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6589" spans="1:5">
+      <c r="A6589">
+        <v>6587</v>
+      </c>
+      <c r="B6589">
+        <v>0</v>
+      </c>
+      <c r="C6589">
+        <v>260</v>
+      </c>
+      <c r="D6589">
+        <v>121</v>
+      </c>
+      <c r="E6589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6590" spans="1:5">
+      <c r="A6590">
+        <v>6588</v>
+      </c>
+      <c r="B6590">
+        <v>0</v>
+      </c>
+      <c r="C6590">
+        <v>261</v>
+      </c>
+      <c r="D6590">
+        <v>121</v>
+      </c>
+      <c r="E6590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6591" spans="1:5">
+      <c r="A6591">
+        <v>6589</v>
+      </c>
+      <c r="B6591">
+        <v>0</v>
+      </c>
+      <c r="C6591">
+        <v>262</v>
+      </c>
+      <c r="D6591">
+        <v>121</v>
+      </c>
+      <c r="E6591">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6592" spans="1:5">
+      <c r="A6592">
+        <v>6590</v>
+      </c>
+      <c r="B6592">
+        <v>0</v>
+      </c>
+      <c r="C6592">
+        <v>263</v>
+      </c>
+      <c r="D6592">
+        <v>121</v>
+      </c>
+      <c r="E6592">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6593" spans="1:5">
+      <c r="A6593">
+        <v>6591</v>
+      </c>
+      <c r="B6593">
+        <v>0</v>
+      </c>
+      <c r="C6593">
+        <v>264</v>
+      </c>
+      <c r="D6593">
+        <v>121</v>
+      </c>
+      <c r="E6593">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6594" spans="1:5">
+      <c r="A6594">
+        <v>6592</v>
+      </c>
+      <c r="B6594">
+        <v>0</v>
+      </c>
+      <c r="C6594">
+        <v>265</v>
+      </c>
+      <c r="D6594">
+        <v>121</v>
+      </c>
+      <c r="E6594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6595" spans="1:5">
+      <c r="A6595">
+        <v>6593</v>
+      </c>
+      <c r="B6595">
+        <v>0</v>
+      </c>
+      <c r="C6595">
+        <v>266</v>
+      </c>
+      <c r="D6595">
+        <v>121</v>
+      </c>
+      <c r="E6595">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6596" spans="1:5">
+      <c r="A6596">
+        <v>6594</v>
+      </c>
+      <c r="B6596">
+        <v>0</v>
+      </c>
+      <c r="C6596">
+        <v>267</v>
+      </c>
+      <c r="D6596">
+        <v>121</v>
+      </c>
+      <c r="E6596">
         <v>0</v>
       </c>
     </row>

</xml_diff>